<commit_message>
[GPR] Atualização do Cronograma do Projeto.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Cronograma Geral do Projeto.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Cronograma Geral do Projeto.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciuscmac/Desktop/GitHub/P.I.-ES-UFG-2015-BIJLMMV/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciuscmac/Desktop/GitHub/P.I.-ES-UFG-2015-BIJLMMV/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="4" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="111">
   <si>
     <t>Atividade</t>
   </si>
@@ -225,9 +225,6 @@
     <t>Gerência de Configuração</t>
   </si>
   <si>
-    <t>Planejar a GCO</t>
-  </si>
-  <si>
     <t>Gerenciar a GCO</t>
   </si>
   <si>
@@ -304,6 +301,84 @@
   </si>
   <si>
     <t>Sala de Reunião</t>
+  </si>
+  <si>
+    <t>Código da Atividade</t>
+  </si>
+  <si>
+    <t>Dependência (cód)</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>Leonardo Freitas / Moisés Hilário / Igor Moura</t>
+  </si>
+  <si>
+    <t>Leonardo Freitas / Moisés Hilário / Breno Fernandes</t>
+  </si>
+  <si>
+    <t>11,12,13</t>
+  </si>
+  <si>
+    <t>Johnathan Gomes</t>
+  </si>
+  <si>
+    <t>Datas do Checklist</t>
+  </si>
+  <si>
+    <t>2 dias úteis</t>
+  </si>
+  <si>
+    <t>Igor Moura / Moisés Hilário</t>
+  </si>
+  <si>
+    <t>Não definido</t>
+  </si>
+  <si>
+    <t>Igor Moura / Vinicius Carvalho</t>
+  </si>
+  <si>
+    <t>Recebimento do PM/RP</t>
+  </si>
+  <si>
+    <t>Equipe de Manutenção</t>
+  </si>
+  <si>
+    <t>Aprovação do PM/RP</t>
+  </si>
+  <si>
+    <t>5 dias úteis</t>
+  </si>
+  <si>
+    <t>Após Implementação</t>
+  </si>
+  <si>
+    <t>1 dia útil</t>
+  </si>
+  <si>
+    <t>Recebimento do Pedido</t>
+  </si>
+  <si>
+    <t>Não Definido</t>
+  </si>
+  <si>
+    <t>Equipe de Configuração / Desenvolvedores</t>
+  </si>
+  <si>
+    <t>Controlar Estado</t>
+  </si>
+  <si>
+    <t>Equipe de Configuração</t>
+  </si>
+  <si>
+    <t>Auditoria da GCO</t>
+  </si>
+  <si>
+    <t>Moisés Hilário / Igor Moura</t>
+  </si>
+  <si>
+    <t>Leonardo Freitas / Igor Moura / Moisés Hilário</t>
   </si>
 </sst>
 </file>
@@ -470,7 +545,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -687,8 +762,14 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF4F81BD"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -855,6 +936,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -916,7 +1047,7 @@
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -935,12 +1066,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -956,34 +1081,52 @@
     <xf numFmtId="0" fontId="21" fillId="36" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1447,10 +1590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J57"/>
+  <dimension ref="B1:L57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1460,13 +1603,16 @@
     <col min="3" max="3" width="26.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" style="1" customWidth="1"/>
     <col min="5" max="6" width="15.5" style="3" customWidth="1"/>
-    <col min="7" max="8" width="19.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" style="3" customWidth="1"/>
     <col min="9" max="9" width="25" style="3" customWidth="1"/>
     <col min="10" max="10" width="25.5" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="1"/>
+    <col min="11" max="11" width="13" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.1640625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C1" s="2"/>
       <c r="D1" s="4"/>
       <c r="G1" s="4"/>
@@ -1474,949 +1620,1654 @@
       <c r="I1" s="4"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="I2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="J2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="K2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="L2" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="16" t="s">
+    <row r="3" spans="2:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="B3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="19">
+        <v>1</v>
+      </c>
+      <c r="E3" s="20">
         <v>42128</v>
       </c>
-      <c r="E3" s="20">
+      <c r="F3" s="20">
         <v>42129</v>
       </c>
-      <c r="F3" s="11">
+      <c r="G3" s="21"/>
+      <c r="H3" s="19">
         <v>3</v>
       </c>
-      <c r="G3" s="21">
+      <c r="I3" s="22">
         <v>1</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="J3" s="24">
+      <c r="J3" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L3" s="23">
         <v>62.4</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="15"/>
-      <c r="C4" s="11" t="s">
+    <row r="4" spans="2:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="B4" s="24"/>
+      <c r="C4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="19">
+        <v>2</v>
+      </c>
+      <c r="E4" s="20">
         <v>42129</v>
       </c>
-      <c r="E4" s="20">
+      <c r="F4" s="20">
         <v>42130</v>
-      </c>
-      <c r="F4" s="11">
-        <v>3</v>
       </c>
       <c r="G4" s="21">
         <v>1</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="J4" s="22">
+      <c r="H4" s="19">
+        <v>3</v>
+      </c>
+      <c r="I4" s="22">
+        <v>1</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L4" s="23">
         <v>62.4</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="15"/>
-      <c r="C5" s="11" t="s">
+    <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="B5" s="24"/>
+      <c r="C5" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="19">
+        <v>3</v>
+      </c>
+      <c r="E5" s="20">
         <v>42130</v>
       </c>
-      <c r="E5" s="20">
+      <c r="F5" s="20">
         <v>42132</v>
       </c>
-      <c r="F5" s="11">
+      <c r="G5" s="21">
+        <v>1.2</v>
+      </c>
+      <c r="H5" s="19">
         <v>6</v>
       </c>
-      <c r="G5" s="21">
+      <c r="I5" s="22">
         <v>1</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="J5" s="22">
+      <c r="J5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" s="23">
         <v>124.8</v>
       </c>
     </row>
-    <row r="6" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="15"/>
-      <c r="C6" s="11" t="s">
+    <row r="6" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B6" s="24"/>
+      <c r="C6" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="19">
+        <v>4</v>
+      </c>
+      <c r="E6" s="20">
         <v>42132</v>
       </c>
-      <c r="E6" s="20">
+      <c r="F6" s="20">
         <v>42135</v>
       </c>
-      <c r="F6" s="11">
+      <c r="G6" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6" s="19">
         <v>9</v>
       </c>
-      <c r="G6" s="21">
+      <c r="I6" s="22">
         <v>1</v>
       </c>
-      <c r="H6" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="J6" s="22">
+      <c r="J6" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L6" s="23">
         <v>187.2</v>
       </c>
     </row>
-    <row r="7" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="15"/>
-      <c r="C7" s="11" t="s">
+    <row r="7" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B7" s="24"/>
+      <c r="C7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="19">
+        <v>5</v>
+      </c>
+      <c r="E7" s="20">
         <v>42128</v>
       </c>
-      <c r="E7" s="20">
+      <c r="F7" s="20">
         <v>42184</v>
       </c>
-      <c r="F7" s="11">
+      <c r="G7" s="21">
+        <v>1</v>
+      </c>
+      <c r="H7" s="19">
         <v>25</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11" t="s">
+      <c r="I7" s="19"/>
+      <c r="J7" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L7" s="23">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B8" s="24"/>
+      <c r="C8" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="19">
+        <v>6</v>
+      </c>
+      <c r="E8" s="20">
+        <v>42128</v>
+      </c>
+      <c r="F8" s="20">
+        <v>42184</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="19">
+        <v>25</v>
+      </c>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L8" s="23">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B9" s="24"/>
+      <c r="C9" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="19">
+        <v>7</v>
+      </c>
+      <c r="E9" s="20">
+        <v>42132</v>
+      </c>
+      <c r="F9" s="20">
+        <v>42135</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="19">
+        <v>9</v>
+      </c>
+      <c r="I9" s="22">
+        <v>1</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K9" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="I7" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="J7" s="22">
+      <c r="L9" s="23">
+        <v>187.2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B10" s="24"/>
+      <c r="C10" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="19">
+        <v>8</v>
+      </c>
+      <c r="E10" s="20">
+        <v>42128</v>
+      </c>
+      <c r="F10" s="20">
+        <v>42184</v>
+      </c>
+      <c r="G10" s="21"/>
+      <c r="H10" s="19">
+        <v>25</v>
+      </c>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="23">
         <v>520</v>
       </c>
     </row>
-    <row r="8" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="15"/>
-      <c r="C8" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="20">
-        <v>42128</v>
-      </c>
-      <c r="E8" s="20">
-        <v>42184</v>
-      </c>
-      <c r="F8" s="11">
-        <v>25</v>
-      </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="J8" s="22">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="15"/>
-      <c r="C9" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="20">
-        <v>42132</v>
-      </c>
-      <c r="E9" s="20">
-        <v>42135</v>
-      </c>
-      <c r="F9" s="11">
+    <row r="11" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B11" s="24"/>
+      <c r="C11" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="19">
         <v>9</v>
-      </c>
-      <c r="G9" s="21">
-        <v>1</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="J9" s="22">
-        <v>187.2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="15"/>
-      <c r="C10" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="20">
-        <v>42128</v>
-      </c>
-      <c r="E10" s="20">
-        <v>42184</v>
-      </c>
-      <c r="F10" s="11">
-        <v>25</v>
-      </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="J10" s="22">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="15"/>
-      <c r="C11" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="20">
-        <v>42131</v>
       </c>
       <c r="E11" s="20">
         <v>42131</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="20">
+        <v>42131</v>
+      </c>
+      <c r="G11" s="21">
+        <v>1.2</v>
+      </c>
+      <c r="H11" s="19">
         <v>3</v>
       </c>
-      <c r="G11" s="21">
+      <c r="I11" s="22">
         <v>1</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="J11" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="23">
+        <v>62.4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B12" s="25"/>
+      <c r="C12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="19">
+        <v>10</v>
+      </c>
+      <c r="E12" s="20">
+        <v>42128</v>
+      </c>
+      <c r="F12" s="20">
+        <v>42184</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="19">
+        <v>24</v>
+      </c>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="I11" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="J11" s="22">
-        <v>62.4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="15"/>
-      <c r="C12" s="11" t="s">
+      <c r="K12" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L12" s="23">
+        <v>499.2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" s="6" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="19">
+        <v>11</v>
+      </c>
+      <c r="E13" s="20">
+        <v>42128</v>
+      </c>
+      <c r="F13" s="20">
+        <v>42129</v>
+      </c>
+      <c r="G13" s="21"/>
+      <c r="H13" s="19">
+        <v>11</v>
+      </c>
+      <c r="I13" s="22">
+        <v>1</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L13" s="23">
+        <v>318.45</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B14" s="14"/>
+      <c r="C14" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="19">
+        <v>12</v>
+      </c>
+      <c r="E14" s="20">
+        <v>42129</v>
+      </c>
+      <c r="F14" s="20">
+        <v>42131</v>
+      </c>
+      <c r="G14" s="21">
+        <v>11</v>
+      </c>
+      <c r="H14" s="19">
+        <v>11</v>
+      </c>
+      <c r="I14" s="22">
+        <v>1</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L14" s="23">
+        <v>318.45</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B15" s="14"/>
+      <c r="C15" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="19">
+        <v>13</v>
+      </c>
+      <c r="E15" s="20">
+        <v>42131</v>
+      </c>
+      <c r="F15" s="20">
+        <v>42133</v>
+      </c>
+      <c r="G15" s="21">
+        <v>11.12</v>
+      </c>
+      <c r="H15" s="19">
+        <v>11</v>
+      </c>
+      <c r="I15" s="22">
+        <v>1</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L15" s="23">
+        <v>318.45</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B16" s="26"/>
+      <c r="C16" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="19">
+        <v>14</v>
+      </c>
+      <c r="E16" s="20">
+        <v>42135</v>
+      </c>
+      <c r="F16" s="20">
+        <v>42184</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="19">
+        <v>33</v>
+      </c>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L16" s="23">
+        <v>955.35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B17" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="19">
+        <v>15</v>
+      </c>
+      <c r="E17" s="20">
+        <v>42130</v>
+      </c>
+      <c r="F17" s="20">
+        <v>42131</v>
+      </c>
+      <c r="G17" s="21">
+        <v>1.2</v>
+      </c>
+      <c r="H17" s="19">
+        <v>6</v>
+      </c>
+      <c r="I17" s="22">
+        <v>1</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L17" s="23">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B18" s="14"/>
+      <c r="C18" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="19">
+        <v>16</v>
+      </c>
+      <c r="E18" s="20">
+        <v>42135</v>
+      </c>
+      <c r="F18" s="20">
+        <v>42184</v>
+      </c>
+      <c r="G18" s="21"/>
+      <c r="H18" s="19">
+        <v>24</v>
+      </c>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L18" s="23">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B19" s="14"/>
+      <c r="C19" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="19">
+        <v>17</v>
+      </c>
+      <c r="E19" s="20">
+        <v>42128</v>
+      </c>
+      <c r="F19" s="20">
+        <v>42184</v>
+      </c>
+      <c r="G19" s="21"/>
+      <c r="H19" s="19">
+        <v>24</v>
+      </c>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L19" s="23">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B20" s="14"/>
+      <c r="C20" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="19">
+        <v>18</v>
+      </c>
+      <c r="E20" s="20">
+        <v>42131</v>
+      </c>
+      <c r="F20" s="20">
+        <v>42132</v>
+      </c>
+      <c r="G20" s="21">
+        <v>15</v>
+      </c>
+      <c r="H20" s="19">
+        <v>6</v>
+      </c>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L20" s="23">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B21" s="14"/>
+      <c r="C21" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="19">
+        <v>19</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21" s="21"/>
+      <c r="H21" s="19">
+        <v>10</v>
+      </c>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L21" s="23">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B22" s="26"/>
+      <c r="C22" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="19">
+        <v>20</v>
+      </c>
+      <c r="E22" s="20">
+        <v>42132</v>
+      </c>
+      <c r="F22" s="20">
+        <v>42135</v>
+      </c>
+      <c r="G22" s="21">
+        <v>15.18</v>
+      </c>
+      <c r="H22" s="19">
+        <v>18</v>
+      </c>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K22" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L22" s="23">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B23" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="19">
+        <v>21</v>
+      </c>
+      <c r="E23" s="20">
+        <v>42128</v>
+      </c>
+      <c r="F23" s="20">
+        <v>42132</v>
+      </c>
+      <c r="G23" s="21"/>
+      <c r="H23" s="19">
+        <v>12</v>
+      </c>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="K23" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L23" s="23">
+        <v>231.96</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B24" s="14"/>
+      <c r="C24" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="19">
+        <v>22</v>
+      </c>
+      <c r="E24" s="20">
+        <v>42135</v>
+      </c>
+      <c r="F24" s="20">
+        <v>42176</v>
+      </c>
+      <c r="G24" s="21">
+        <v>12.21</v>
+      </c>
+      <c r="H24" s="19">
+        <v>24</v>
+      </c>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="K24" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L24" s="23">
+        <v>463.92</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B25" s="14"/>
+      <c r="C25" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="19">
+        <v>23</v>
+      </c>
+      <c r="E25" s="20">
+        <v>42135</v>
+      </c>
+      <c r="F25" s="20">
+        <v>42176</v>
+      </c>
+      <c r="G25" s="21">
+        <v>21.49</v>
+      </c>
+      <c r="H25" s="19">
+        <v>24</v>
+      </c>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="K25" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L25" s="23">
+        <v>463.92</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B26" s="14"/>
+      <c r="C26" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="19">
+        <v>24</v>
+      </c>
+      <c r="E26" s="20">
+        <v>42142</v>
+      </c>
+      <c r="F26" s="20">
+        <v>42184</v>
+      </c>
+      <c r="G26" s="21">
+        <v>21.38</v>
+      </c>
+      <c r="H26" s="19">
+        <v>24</v>
+      </c>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="K26" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L26" s="23">
+        <v>463.92</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B27" s="14"/>
+      <c r="C27" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="19">
+        <v>25</v>
+      </c>
+      <c r="E27" s="28">
+        <v>42142</v>
+      </c>
+      <c r="F27" s="20">
+        <v>42184</v>
+      </c>
+      <c r="G27" s="21">
+        <v>24</v>
+      </c>
+      <c r="H27" s="19">
+        <v>24</v>
+      </c>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="K27" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L27" s="23">
+        <v>463.92</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B28" s="26"/>
+      <c r="C28" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="19">
+        <v>26</v>
+      </c>
+      <c r="E28" s="20">
+        <v>42135</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" s="21">
+        <v>21.3</v>
+      </c>
+      <c r="H28" s="19">
+        <v>24</v>
+      </c>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="K28" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L28" s="23">
+        <v>463.92</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B29" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="19">
+        <v>27</v>
+      </c>
+      <c r="E29" s="20">
+        <v>42191</v>
+      </c>
+      <c r="F29" s="20">
+        <v>42135</v>
+      </c>
+      <c r="G29" s="21">
+        <v>1.2</v>
+      </c>
+      <c r="H29" s="19">
+        <v>14</v>
+      </c>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="K29" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L29" s="23">
+        <v>158.30000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B30" s="14"/>
+      <c r="C30" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="19">
+        <v>28</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G30" s="21"/>
+      <c r="H30" s="19">
+        <v>24</v>
+      </c>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="K30" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L30" s="23">
+        <v>271.2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B31" s="14"/>
+      <c r="C31" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="19">
+        <v>29</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G31" s="21">
+        <v>28</v>
+      </c>
+      <c r="H31" s="19">
+        <v>44</v>
+      </c>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="K31" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L31" s="23">
+        <v>497.2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B32" s="14"/>
+      <c r="C32" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="19">
+        <v>30</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G32" s="21">
+        <v>28.29</v>
+      </c>
+      <c r="H32" s="19">
+        <v>6</v>
+      </c>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="K32" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L32" s="23">
+        <v>67.8</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B33" s="14"/>
+      <c r="C33" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="19">
         <v>31</v>
       </c>
-      <c r="D12" s="20">
+      <c r="E33" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" s="21"/>
+      <c r="H33" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="K33" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L33" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B34" s="26"/>
+      <c r="C34" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="19">
+        <v>32</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G34" s="21"/>
+      <c r="H34" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="K34" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L34" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="19">
+        <v>33</v>
+      </c>
+      <c r="E35" s="20">
         <v>42128</v>
       </c>
-      <c r="E12" s="20">
+      <c r="F35" s="20">
+        <v>42130</v>
+      </c>
+      <c r="G35" s="21"/>
+      <c r="H35" s="19">
+        <v>8</v>
+      </c>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="K35" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L35" s="23">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B36" s="14"/>
+      <c r="C36" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="19">
+        <v>34</v>
+      </c>
+      <c r="E36" s="20">
+        <v>42130</v>
+      </c>
+      <c r="F36" s="20">
+        <v>42133</v>
+      </c>
+      <c r="G36" s="21">
+        <v>33</v>
+      </c>
+      <c r="H36" s="19">
+        <v>8</v>
+      </c>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="K36" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L36" s="23">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B37" s="14"/>
+      <c r="C37" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="19">
+        <v>35</v>
+      </c>
+      <c r="E37" s="20">
+        <v>42135</v>
+      </c>
+      <c r="F37" s="20">
         <v>42184</v>
       </c>
-      <c r="F12" s="11">
-        <v>24</v>
-      </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11" t="s">
+      <c r="G37" s="21">
+        <v>33.340000000000003</v>
+      </c>
+      <c r="H37" s="19">
+        <v>10</v>
+      </c>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="K37" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L37" s="23">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B38" s="14"/>
+      <c r="C38" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" s="19">
+        <v>36</v>
+      </c>
+      <c r="E38" s="20">
+        <v>42135</v>
+      </c>
+      <c r="F38" s="20">
+        <v>42184</v>
+      </c>
+      <c r="G38" s="21">
+        <v>33.340000000000003</v>
+      </c>
+      <c r="H38" s="19">
+        <v>8</v>
+      </c>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="K38" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L38" s="23">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B39" s="26"/>
+      <c r="C39" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D39" s="19">
+        <v>37</v>
+      </c>
+      <c r="E39" s="20">
+        <v>42135</v>
+      </c>
+      <c r="F39" s="20">
+        <v>42184</v>
+      </c>
+      <c r="G39" s="21">
+        <v>33.340000000000003</v>
+      </c>
+      <c r="H39" s="19">
+        <v>10</v>
+      </c>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K39" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L39" s="23">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B40" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" s="19">
+        <v>38</v>
+      </c>
+      <c r="E40" s="20">
+        <v>42135</v>
+      </c>
+      <c r="F40" s="20">
+        <v>42142</v>
+      </c>
+      <c r="G40" s="21"/>
+      <c r="H40" s="19">
+        <v>11</v>
+      </c>
+      <c r="I40" s="22">
+        <v>1</v>
+      </c>
+      <c r="J40" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="K40" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L40" s="23">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B41" s="14"/>
+      <c r="C41" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="19">
+        <v>39</v>
+      </c>
+      <c r="E41" s="20">
+        <v>42135</v>
+      </c>
+      <c r="F41" s="20">
+        <v>42142</v>
+      </c>
+      <c r="G41" s="21">
+        <v>38</v>
+      </c>
+      <c r="H41" s="19">
+        <v>11</v>
+      </c>
+      <c r="I41" s="22">
+        <v>1</v>
+      </c>
+      <c r="J41" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="K41" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L41" s="23">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B42" s="14"/>
+      <c r="C42" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="19">
+        <v>40</v>
+      </c>
+      <c r="E42" s="20">
+        <v>42135</v>
+      </c>
+      <c r="F42" s="20">
+        <v>42142</v>
+      </c>
+      <c r="G42" s="21">
+        <v>39</v>
+      </c>
+      <c r="H42" s="19">
+        <v>11</v>
+      </c>
+      <c r="I42" s="22">
+        <v>1</v>
+      </c>
+      <c r="J42" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="K42" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L42" s="23">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="B43" s="14"/>
+      <c r="C43" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" s="19">
+        <v>41</v>
+      </c>
+      <c r="E43" s="20">
+        <v>42135</v>
+      </c>
+      <c r="F43" s="20">
+        <v>42142</v>
+      </c>
+      <c r="G43" s="21">
+        <v>40</v>
+      </c>
+      <c r="H43" s="19">
+        <v>11</v>
+      </c>
+      <c r="I43" s="22">
+        <v>1</v>
+      </c>
+      <c r="J43" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="K43" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L43" s="23">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B44" s="14"/>
+      <c r="C44" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="19">
+        <v>42</v>
+      </c>
+      <c r="E44" s="20">
+        <v>42149</v>
+      </c>
+      <c r="F44" s="20">
+        <v>42156</v>
+      </c>
+      <c r="G44" s="21">
+        <v>41</v>
+      </c>
+      <c r="H44" s="19">
+        <v>11</v>
+      </c>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="K44" s="19"/>
+      <c r="L44" s="23">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B45" s="14"/>
+      <c r="C45" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" s="19">
+        <v>43</v>
+      </c>
+      <c r="E45" s="20">
+        <v>42149</v>
+      </c>
+      <c r="F45" s="20">
+        <v>42156</v>
+      </c>
+      <c r="G45" s="21">
+        <v>42</v>
+      </c>
+      <c r="H45" s="19">
+        <v>11</v>
+      </c>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="K45" s="19"/>
+      <c r="L45" s="23">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B46" s="14"/>
+      <c r="C46" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" s="19">
+        <v>44</v>
+      </c>
+      <c r="E46" s="20">
+        <v>42149</v>
+      </c>
+      <c r="F46" s="20">
+        <v>42156</v>
+      </c>
+      <c r="G46" s="21">
+        <v>43</v>
+      </c>
+      <c r="H46" s="19">
+        <v>11</v>
+      </c>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="K46" s="19"/>
+      <c r="L46" s="23">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B47" s="14"/>
+      <c r="C47" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" s="19">
+        <v>45</v>
+      </c>
+      <c r="E47" s="20">
+        <v>42149</v>
+      </c>
+      <c r="F47" s="20">
+        <v>42156</v>
+      </c>
+      <c r="G47" s="21">
+        <v>44</v>
+      </c>
+      <c r="H47" s="19">
+        <v>11</v>
+      </c>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="K47" s="19"/>
+      <c r="L47" s="23">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B48" s="14"/>
+      <c r="C48" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48" s="19">
+        <v>46</v>
+      </c>
+      <c r="E48" s="20">
+        <v>42163</v>
+      </c>
+      <c r="F48" s="20">
+        <v>42170</v>
+      </c>
+      <c r="G48" s="21">
+        <v>45</v>
+      </c>
+      <c r="H48" s="19">
+        <v>22</v>
+      </c>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="K48" s="19"/>
+      <c r="L48" s="23">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B49" s="14"/>
+      <c r="C49" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D49" s="19">
+        <v>47</v>
+      </c>
+      <c r="E49" s="20">
+        <v>42163</v>
+      </c>
+      <c r="F49" s="20">
+        <v>42170</v>
+      </c>
+      <c r="G49" s="21">
+        <v>46</v>
+      </c>
+      <c r="H49" s="19">
+        <v>22</v>
+      </c>
+      <c r="I49" s="19"/>
+      <c r="J49" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="K49" s="19"/>
+      <c r="L49" s="23">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B50" s="26"/>
+      <c r="C50" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" s="19">
+        <v>48</v>
+      </c>
+      <c r="E50" s="20">
+        <v>42177</v>
+      </c>
+      <c r="F50" s="20">
+        <v>42184</v>
+      </c>
+      <c r="G50" s="21">
+        <v>47</v>
+      </c>
+      <c r="H50" s="19">
+        <v>44</v>
+      </c>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="K50" s="19"/>
+      <c r="L50" s="23">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B51" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51" s="19">
+        <v>49</v>
+      </c>
+      <c r="E51" s="20">
+        <v>42132</v>
+      </c>
+      <c r="F51" s="20">
+        <v>42135</v>
+      </c>
+      <c r="G51" s="21">
+        <v>1.2</v>
+      </c>
+      <c r="H51" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="K51" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="I12" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="J12" s="22">
-        <v>499.2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" s="6" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="18"/>
-      <c r="C14" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-    </row>
-    <row r="15" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="18"/>
-      <c r="C15" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-    </row>
-    <row r="16" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="19"/>
-      <c r="C16" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-    </row>
-    <row r="17" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-    </row>
-    <row r="18" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="18"/>
-      <c r="C18" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-    </row>
-    <row r="19" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="18"/>
-      <c r="C19" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-    </row>
-    <row r="20" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="18"/>
-      <c r="C20" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-    </row>
-    <row r="21" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="18"/>
-      <c r="C21" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-    </row>
-    <row r="22" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="19"/>
-      <c r="C22" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-    </row>
-    <row r="23" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-    </row>
-    <row r="24" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="18"/>
-      <c r="C24" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-    </row>
-    <row r="25" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="18"/>
-      <c r="C25" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-    </row>
-    <row r="26" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="18"/>
-      <c r="C26" s="11" t="s">
+      <c r="L51" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B52" s="14"/>
+      <c r="C52" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D52" s="19">
+        <v>50</v>
+      </c>
+      <c r="E52" s="20">
+        <v>42135</v>
+      </c>
+      <c r="F52" s="20">
+        <v>42176</v>
+      </c>
+      <c r="G52" s="21">
         <v>48</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-    </row>
-    <row r="27" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="18"/>
-      <c r="C27" s="11" t="s">
+      <c r="H52" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="K52" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L52" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="B53" s="26"/>
+      <c r="C53" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="19">
+        <v>51</v>
+      </c>
+      <c r="E53" s="20">
+        <v>42135</v>
+      </c>
+      <c r="F53" s="20">
+        <v>42176</v>
+      </c>
+      <c r="G53" s="21">
         <v>49</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-    </row>
-    <row r="28" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="19"/>
-      <c r="C28" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-    </row>
-    <row r="29" spans="2:10" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="B29" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-    </row>
-    <row r="30" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="18"/>
-      <c r="C30" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-    </row>
-    <row r="31" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="18"/>
-      <c r="C31" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-    </row>
-    <row r="32" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B32" s="18"/>
-      <c r="C32" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-    </row>
-    <row r="33" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="18"/>
-      <c r="C33" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-    </row>
-    <row r="34" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="19"/>
-      <c r="C34" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-    </row>
-    <row r="35" spans="2:10" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B35" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-    </row>
-    <row r="36" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="18"/>
-      <c r="C36" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-    </row>
-    <row r="37" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="18"/>
-      <c r="C37" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-    </row>
-    <row r="38" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B38" s="19"/>
-      <c r="C38" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-    </row>
-    <row r="39" spans="2:10" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B39" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" s="20">
-        <v>42135</v>
-      </c>
-      <c r="E39" s="20">
-        <v>42142</v>
-      </c>
-      <c r="F39" s="11">
-        <v>11</v>
-      </c>
-      <c r="G39" s="21">
-        <v>1</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="J39" s="22">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B40" s="18"/>
-      <c r="C40" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="20">
-        <v>42135</v>
-      </c>
-      <c r="E40" s="20">
-        <v>42142</v>
-      </c>
-      <c r="F40" s="11">
-        <v>11</v>
-      </c>
-      <c r="G40" s="21">
-        <v>1</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="J40" s="22">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B41" s="18"/>
-      <c r="C41" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D41" s="20">
-        <v>42135</v>
-      </c>
-      <c r="E41" s="20">
-        <v>42142</v>
-      </c>
-      <c r="F41" s="11">
-        <v>11</v>
-      </c>
-      <c r="G41" s="21">
-        <v>1</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I41" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="J41" s="22">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B42" s="18"/>
-      <c r="C42" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D42" s="20">
-        <v>42135</v>
-      </c>
-      <c r="E42" s="20">
-        <v>42142</v>
-      </c>
-      <c r="F42" s="11">
-        <v>11</v>
-      </c>
-      <c r="G42" s="21">
-        <v>1</v>
-      </c>
-      <c r="H42" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="I42" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="J42" s="22">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B43" s="18"/>
-      <c r="C43" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43" s="20">
-        <v>42149</v>
-      </c>
-      <c r="E43" s="20">
-        <v>42156</v>
-      </c>
-      <c r="F43" s="11">
-        <v>11</v>
-      </c>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11"/>
-    </row>
-    <row r="44" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B44" s="18"/>
-      <c r="C44" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D44" s="20">
-        <v>42149</v>
-      </c>
-      <c r="E44" s="20">
-        <v>42156</v>
-      </c>
-      <c r="F44" s="11">
-        <v>11</v>
-      </c>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
-    </row>
-    <row r="45" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B45" s="18"/>
-      <c r="C45" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D45" s="20">
-        <v>42149</v>
-      </c>
-      <c r="E45" s="20">
-        <v>42156</v>
-      </c>
-      <c r="F45" s="11">
-        <v>11</v>
-      </c>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-    </row>
-    <row r="46" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B46" s="18"/>
-      <c r="C46" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D46" s="20">
-        <v>42149</v>
-      </c>
-      <c r="E46" s="20">
-        <v>42156</v>
-      </c>
-      <c r="F46" s="11">
-        <v>11</v>
-      </c>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-    </row>
-    <row r="47" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B47" s="18"/>
-      <c r="C47" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D47" s="20">
-        <v>42163</v>
-      </c>
-      <c r="E47" s="20">
-        <v>42170</v>
-      </c>
-      <c r="F47" s="11">
-        <v>22</v>
-      </c>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-    </row>
-    <row r="48" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B48" s="18"/>
-      <c r="C48" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D48" s="20">
-        <v>42163</v>
-      </c>
-      <c r="E48" s="20">
-        <v>42170</v>
-      </c>
-      <c r="F48" s="11">
-        <v>22</v>
-      </c>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-    </row>
-    <row r="49" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B49" s="19"/>
-      <c r="C49" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D49" s="20">
-        <v>42177</v>
-      </c>
-      <c r="E49" s="20">
-        <v>42184</v>
-      </c>
-      <c r="F49" s="11">
-        <v>44</v>
-      </c>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-    </row>
-    <row r="50" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B50" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-    </row>
-    <row r="51" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B51" s="18"/>
-      <c r="C51" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-    </row>
-    <row r="52" spans="2:10" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="B52" s="19"/>
-      <c r="C52" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H53" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="I53" s="19"/>
+      <c r="J53" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="K53" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L53" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C56" s="7"/>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C57" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B39:B49"/>
-    <mergeCell ref="B50:B52"/>
     <mergeCell ref="B3:B12"/>
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="B17:B22"/>
     <mergeCell ref="B23:B28"/>
     <mergeCell ref="B29:B34"/>
-    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B35:B39"/>
+    <mergeCell ref="B40:B50"/>
+    <mergeCell ref="B51:B53"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="I2:I53">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="percentile" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="100"/>
+        <color rgb="FFC00000"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF92D050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.31496062992125984" right="0.35433070866141736" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -2446,58 +3297,58 @@
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:3" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:3" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:3" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[GPR] Atualizando porcentagens do cronograma.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Cronograma Geral do Projeto.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Cronograma Geral do Projeto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25924"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1108,6 +1108,15 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1120,75 +1129,66 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="58">
+    <cellStyle name="Accent1" xfId="1" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent1 - 20%" xfId="2"/>
     <cellStyle name="Accent1 - 20% 2" xfId="45"/>
     <cellStyle name="Accent1 - 40%" xfId="3"/>
     <cellStyle name="Accent1 - 40% 2" xfId="46"/>
     <cellStyle name="Accent1 - 60%" xfId="4"/>
+    <cellStyle name="Accent2" xfId="5" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent2 - 20%" xfId="6"/>
     <cellStyle name="Accent2 - 20% 2" xfId="47"/>
     <cellStyle name="Accent2 - 40%" xfId="7"/>
     <cellStyle name="Accent2 - 40% 2" xfId="48"/>
     <cellStyle name="Accent2 - 60%" xfId="8"/>
+    <cellStyle name="Accent3" xfId="9" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent3 - 20%" xfId="10"/>
     <cellStyle name="Accent3 - 20% 2" xfId="49"/>
     <cellStyle name="Accent3 - 40%" xfId="11"/>
     <cellStyle name="Accent3 - 40% 2" xfId="50"/>
     <cellStyle name="Accent3 - 60%" xfId="12"/>
+    <cellStyle name="Accent4" xfId="13" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent4 - 20%" xfId="14"/>
     <cellStyle name="Accent4 - 20% 2" xfId="51"/>
     <cellStyle name="Accent4 - 40%" xfId="15"/>
     <cellStyle name="Accent4 - 40% 2" xfId="52"/>
     <cellStyle name="Accent4 - 60%" xfId="16"/>
+    <cellStyle name="Accent5" xfId="17" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent5 - 20%" xfId="18"/>
     <cellStyle name="Accent5 - 20% 2" xfId="53"/>
     <cellStyle name="Accent5 - 40%" xfId="19"/>
     <cellStyle name="Accent5 - 40% 2" xfId="54"/>
     <cellStyle name="Accent5 - 60%" xfId="20"/>
+    <cellStyle name="Accent6" xfId="21" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Accent6 - 20%" xfId="22"/>
     <cellStyle name="Accent6 - 20% 2" xfId="55"/>
     <cellStyle name="Accent6 - 40%" xfId="23"/>
     <cellStyle name="Accent6 - 40% 2" xfId="56"/>
     <cellStyle name="Accent6 - 60%" xfId="24"/>
-    <cellStyle name="Bom" xfId="31" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Célula Vinculada" xfId="37" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Emphasis 1" xfId="28"/>
     <cellStyle name="Emphasis 2" xfId="29"/>
     <cellStyle name="Emphasis 3" xfId="30"/>
-    <cellStyle name="Ênfase1" xfId="1" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Ênfase2" xfId="5" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Ênfase3" xfId="9" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Ênfase4" xfId="13" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Ênfase5" xfId="17" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Ênfase6" xfId="21" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="36" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorreto" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutra" xfId="38" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="31" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="32" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="33" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="35" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="36" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="37" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="38" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="44"/>
-    <cellStyle name="Observação" xfId="39" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="39" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="40" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Percent 2" xfId="57"/>
-    <cellStyle name="Saída" xfId="40" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Sheet Title" xfId="41"/>
-    <cellStyle name="Texto de Aviso" xfId="43" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="32" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="33" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="34" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Título 4" xfId="35" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Verificar Célula" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1592,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" zoomScale="101" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1656,7 +1656,7 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="16" t="s">
@@ -1689,7 +1689,7 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="23"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="16" t="s">
         <v>23</v>
       </c>
@@ -1722,7 +1722,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="23"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="16" t="s">
         <v>30</v>
       </c>
@@ -1755,7 +1755,7 @@
       </c>
     </row>
     <row r="6" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="23"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="16" t="s">
         <v>24</v>
       </c>
@@ -1788,7 +1788,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B7" s="23"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="16" t="s">
         <v>25</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>25</v>
       </c>
       <c r="I7" s="19">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="J7" s="16" t="s">
         <v>82</v>
@@ -1821,7 +1821,7 @@
       </c>
     </row>
     <row r="8" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B8" s="23"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="16" t="s">
         <v>26</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>25</v>
       </c>
       <c r="I8" s="19">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="J8" s="16" t="s">
         <v>82</v>
@@ -1852,7 +1852,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="23"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="16" t="s">
         <v>27</v>
       </c>
@@ -1885,7 +1885,7 @@
       </c>
     </row>
     <row r="10" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B10" s="23"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="16" t="s">
         <v>28</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>25</v>
       </c>
       <c r="I10" s="19">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="J10" s="16" t="s">
         <v>82</v>
@@ -1916,7 +1916,7 @@
       </c>
     </row>
     <row r="11" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="23"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="16" t="s">
         <v>29</v>
       </c>
@@ -1949,7 +1949,7 @@
       </c>
     </row>
     <row r="12" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B12" s="24"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="16" t="s">
         <v>31</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>24</v>
       </c>
       <c r="I12" s="19">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="J12" s="16" t="s">
         <v>82</v>
@@ -1980,7 +1980,7 @@
       </c>
     </row>
     <row r="13" spans="2:12" s="6" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="28" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="16" t="s">
@@ -2013,7 +2013,7 @@
       </c>
     </row>
     <row r="14" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="B14" s="26"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="16" t="s">
         <v>33</v>
       </c>
@@ -2046,7 +2046,7 @@
       </c>
     </row>
     <row r="15" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B15" s="26"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="16" t="s">
         <v>34</v>
       </c>
@@ -2079,7 +2079,7 @@
       </c>
     </row>
     <row r="16" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B16" s="27"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="16" t="s">
         <v>35</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>33</v>
       </c>
       <c r="I16" s="19">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="J16" s="16" t="s">
         <v>77</v>
@@ -2112,7 +2112,7 @@
       </c>
     </row>
     <row r="17" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="22" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="16" t="s">
@@ -2147,7 +2147,7 @@
       </c>
     </row>
     <row r="18" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B18" s="26"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="16" t="s">
         <v>39</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>24</v>
       </c>
       <c r="I18" s="19">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="J18" s="16" t="s">
         <v>90</v>
@@ -2178,7 +2178,7 @@
       </c>
     </row>
     <row r="19" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B19" s="26"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="16" t="s">
         <v>40</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>24</v>
       </c>
       <c r="I19" s="19">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="J19" s="16" t="s">
         <v>90</v>
@@ -2209,7 +2209,7 @@
       </c>
     </row>
     <row r="20" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="26"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="16" t="s">
         <v>41</v>
       </c>
@@ -2242,7 +2242,7 @@
       </c>
     </row>
     <row r="21" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="26"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="16" t="s">
         <v>42</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>10</v>
       </c>
       <c r="I21" s="19">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="J21" s="16" t="s">
         <v>90</v>
@@ -2273,7 +2273,7 @@
       </c>
     </row>
     <row r="22" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="27"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="16" t="s">
         <v>43</v>
       </c>
@@ -2306,7 +2306,7 @@
       </c>
     </row>
     <row r="23" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="22" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="16" t="s">
@@ -2339,7 +2339,7 @@
       </c>
     </row>
     <row r="24" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B24" s="26"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="16" t="s">
         <v>46</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>24</v>
       </c>
       <c r="I24" s="19">
-        <v>0.25</v>
+        <v>0.6</v>
       </c>
       <c r="J24" s="16" t="s">
         <v>93</v>
@@ -2372,7 +2372,7 @@
       </c>
     </row>
     <row r="25" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B25" s="26"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="16" t="s">
         <v>47</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>24</v>
       </c>
       <c r="I25" s="19">
-        <v>0.25</v>
+        <v>0.6</v>
       </c>
       <c r="J25" s="16" t="s">
         <v>93</v>
@@ -2405,7 +2405,7 @@
       </c>
     </row>
     <row r="26" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B26" s="26"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="16" t="s">
         <v>48</v>
       </c>
@@ -2438,7 +2438,7 @@
       </c>
     </row>
     <row r="27" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B27" s="27"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="16" t="s">
         <v>49</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>24</v>
       </c>
       <c r="I27" s="19">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="J27" s="16" t="s">
         <v>93</v>
@@ -2471,7 +2471,7 @@
       </c>
     </row>
     <row r="28" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="22" t="s">
         <v>50</v>
       </c>
       <c r="C28" s="16" t="s">
@@ -2506,7 +2506,7 @@
       </c>
     </row>
     <row r="29" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="B29" s="26"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="16" t="s">
         <v>52</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>24</v>
       </c>
       <c r="I29" s="19">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="J29" s="16" t="s">
         <v>80</v>
@@ -2537,7 +2537,7 @@
       </c>
     </row>
     <row r="30" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B30" s="26"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="16" t="s">
         <v>53</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>44</v>
       </c>
       <c r="I30" s="19">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="J30" s="16" t="s">
         <v>97</v>
@@ -2570,7 +2570,7 @@
       </c>
     </row>
     <row r="31" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="B31" s="26"/>
+      <c r="B31" s="23"/>
       <c r="C31" s="16" t="s">
         <v>54</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>6</v>
       </c>
       <c r="I31" s="19">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="J31" s="16" t="s">
         <v>77</v>
@@ -2603,7 +2603,7 @@
       </c>
     </row>
     <row r="32" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B32" s="26"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="16" t="s">
         <v>55</v>
       </c>
@@ -2634,7 +2634,7 @@
       </c>
     </row>
     <row r="33" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B33" s="27"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="16" t="s">
         <v>56</v>
       </c>
@@ -2665,7 +2665,7 @@
       </c>
     </row>
     <row r="34" spans="2:12" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="22" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="16" t="s">
@@ -2698,7 +2698,7 @@
       </c>
     </row>
     <row r="35" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B35" s="26"/>
+      <c r="B35" s="23"/>
       <c r="C35" s="16" t="s">
         <v>59</v>
       </c>
@@ -2731,7 +2731,7 @@
       </c>
     </row>
     <row r="36" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B36" s="26"/>
+      <c r="B36" s="23"/>
       <c r="C36" s="16" t="s">
         <v>35</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>10</v>
       </c>
       <c r="I36" s="19">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="J36" s="16" t="s">
         <v>104</v>
@@ -2764,7 +2764,7 @@
       </c>
     </row>
     <row r="37" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B37" s="26"/>
+      <c r="B37" s="23"/>
       <c r="C37" s="16" t="s">
         <v>105</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>8</v>
       </c>
       <c r="I37" s="19">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="J37" s="16" t="s">
         <v>106</v>
@@ -2797,7 +2797,7 @@
       </c>
     </row>
     <row r="38" spans="2:12" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B38" s="27"/>
+      <c r="B38" s="24"/>
       <c r="C38" s="16" t="s">
         <v>107</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>10</v>
       </c>
       <c r="I38" s="19">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="J38" s="16" t="s">
         <v>80</v>
@@ -2830,7 +2830,7 @@
       </c>
     </row>
     <row r="39" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="22" t="s">
         <v>60</v>
       </c>
       <c r="C39" s="16" t="s">
@@ -2863,7 +2863,7 @@
       </c>
     </row>
     <row r="40" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B40" s="26"/>
+      <c r="B40" s="23"/>
       <c r="C40" s="16" t="s">
         <v>62</v>
       </c>
@@ -2896,7 +2896,7 @@
       </c>
     </row>
     <row r="41" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B41" s="26"/>
+      <c r="B41" s="23"/>
       <c r="C41" s="16" t="s">
         <v>63</v>
       </c>
@@ -2929,7 +2929,7 @@
       </c>
     </row>
     <row r="42" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B42" s="26"/>
+      <c r="B42" s="23"/>
       <c r="C42" s="16" t="s">
         <v>64</v>
       </c>
@@ -2962,7 +2962,7 @@
       </c>
     </row>
     <row r="43" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B43" s="26"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="16" t="s">
         <v>65</v>
       </c>
@@ -2993,7 +2993,7 @@
       </c>
     </row>
     <row r="44" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B44" s="26"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="16" t="s">
         <v>66</v>
       </c>
@@ -3024,7 +3024,7 @@
       </c>
     </row>
     <row r="45" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B45" s="26"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="16" t="s">
         <v>67</v>
       </c>
@@ -3055,7 +3055,7 @@
       </c>
     </row>
     <row r="46" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B46" s="26"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="16" t="s">
         <v>68</v>
       </c>
@@ -3086,7 +3086,7 @@
       </c>
     </row>
     <row r="47" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B47" s="26"/>
+      <c r="B47" s="23"/>
       <c r="C47" s="16" t="s">
         <v>69</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>22</v>
       </c>
       <c r="I47" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" s="16" t="s">
         <v>108</v>
@@ -3117,7 +3117,7 @@
       </c>
     </row>
     <row r="48" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B48" s="26"/>
+      <c r="B48" s="23"/>
       <c r="C48" s="16" t="s">
         <v>70</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>22</v>
       </c>
       <c r="I48" s="19">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J48" s="16" t="s">
         <v>76</v>
@@ -3148,7 +3148,7 @@
       </c>
     </row>
     <row r="49" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="B49" s="27"/>
+      <c r="B49" s="24"/>
       <c r="C49" s="16" t="s">
         <v>71</v>
       </c>
@@ -3179,7 +3179,7 @@
       </c>
     </row>
     <row r="50" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="B50" s="28" t="s">
+      <c r="B50" s="22" t="s">
         <v>72</v>
       </c>
       <c r="C50" s="16" t="s">
@@ -3214,7 +3214,7 @@
       </c>
     </row>
     <row r="51" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="B51" s="26"/>
+      <c r="B51" s="23"/>
       <c r="C51" s="16" t="s">
         <v>74</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>103</v>
       </c>
       <c r="I51" s="19">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="J51" s="16" t="s">
         <v>87</v>
@@ -3247,7 +3247,7 @@
       </c>
     </row>
     <row r="52" spans="2:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="B52" s="27"/>
+      <c r="B52" s="24"/>
       <c r="C52" s="16" t="s">
         <v>75</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>103</v>
       </c>
       <c r="I52" s="19">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="J52" s="16" t="s">
         <v>87</v>
@@ -3294,7 +3294,7 @@
       </c>
       <c r="I53" s="19">
         <f>AVERAGE(I3:I52)</f>
-        <v>0.64699999999999991</v>
+        <v>0.7659999999999999</v>
       </c>
       <c r="J53" s="16"/>
       <c r="K53" s="16"/>

</xml_diff>

<commit_message>
[GPR] Atualizando porcentagem do Cronograma.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Cronograma Geral do Projeto.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Cronograma Geral do Projeto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25924"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25908"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1131,64 +1131,64 @@
     </xf>
   </cellXfs>
   <cellStyles count="58">
-    <cellStyle name="Accent1" xfId="1" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent1 - 20%" xfId="2"/>
     <cellStyle name="Accent1 - 20% 2" xfId="45"/>
     <cellStyle name="Accent1 - 40%" xfId="3"/>
     <cellStyle name="Accent1 - 40% 2" xfId="46"/>
     <cellStyle name="Accent1 - 60%" xfId="4"/>
-    <cellStyle name="Accent2" xfId="5" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent2 - 20%" xfId="6"/>
     <cellStyle name="Accent2 - 20% 2" xfId="47"/>
     <cellStyle name="Accent2 - 40%" xfId="7"/>
     <cellStyle name="Accent2 - 40% 2" xfId="48"/>
     <cellStyle name="Accent2 - 60%" xfId="8"/>
-    <cellStyle name="Accent3" xfId="9" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent3 - 20%" xfId="10"/>
     <cellStyle name="Accent3 - 20% 2" xfId="49"/>
     <cellStyle name="Accent3 - 40%" xfId="11"/>
     <cellStyle name="Accent3 - 40% 2" xfId="50"/>
     <cellStyle name="Accent3 - 60%" xfId="12"/>
-    <cellStyle name="Accent4" xfId="13" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent4 - 20%" xfId="14"/>
     <cellStyle name="Accent4 - 20% 2" xfId="51"/>
     <cellStyle name="Accent4 - 40%" xfId="15"/>
     <cellStyle name="Accent4 - 40% 2" xfId="52"/>
     <cellStyle name="Accent4 - 60%" xfId="16"/>
-    <cellStyle name="Accent5" xfId="17" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent5 - 20%" xfId="18"/>
     <cellStyle name="Accent5 - 20% 2" xfId="53"/>
     <cellStyle name="Accent5 - 40%" xfId="19"/>
     <cellStyle name="Accent5 - 40% 2" xfId="54"/>
     <cellStyle name="Accent5 - 60%" xfId="20"/>
-    <cellStyle name="Accent6" xfId="21" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Accent6 - 20%" xfId="22"/>
     <cellStyle name="Accent6 - 20% 2" xfId="55"/>
     <cellStyle name="Accent6 - 40%" xfId="23"/>
     <cellStyle name="Accent6 - 40% 2" xfId="56"/>
     <cellStyle name="Accent6 - 60%" xfId="24"/>
-    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Bom" xfId="31" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Célula Vinculada" xfId="37" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Emphasis 1" xfId="28"/>
     <cellStyle name="Emphasis 2" xfId="29"/>
     <cellStyle name="Emphasis 3" xfId="30"/>
-    <cellStyle name="Good" xfId="31" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="32" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="33" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="35" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="36" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="37" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="38" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Ênfase1" xfId="1" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Ênfase2" xfId="5" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Ênfase3" xfId="9" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Ênfase4" xfId="13" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Ênfase5" xfId="17" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Ênfase6" xfId="21" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="36" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorreto" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutra" xfId="38" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="44"/>
-    <cellStyle name="Note" xfId="39" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="40" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Observação" xfId="39" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Percent 2" xfId="57"/>
+    <cellStyle name="Saída" xfId="40" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Sheet Title" xfId="41"/>
+    <cellStyle name="Texto de Aviso" xfId="43" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="32" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="33" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="34" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Título 4" xfId="35" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Verificar Célula" xfId="27" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1592,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A87" zoomScale="101" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1808,7 +1808,7 @@
         <v>25</v>
       </c>
       <c r="I7" s="19">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J7" s="16" t="s">
         <v>82</v>
@@ -1839,7 +1839,7 @@
         <v>25</v>
       </c>
       <c r="I8" s="19">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J8" s="16" t="s">
         <v>82</v>
@@ -1903,7 +1903,7 @@
         <v>25</v>
       </c>
       <c r="I10" s="19">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J10" s="16" t="s">
         <v>82</v>
@@ -1967,7 +1967,7 @@
         <v>24</v>
       </c>
       <c r="I12" s="19">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J12" s="16" t="s">
         <v>82</v>
@@ -2099,7 +2099,7 @@
         <v>33</v>
       </c>
       <c r="I16" s="19">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J16" s="16" t="s">
         <v>77</v>
@@ -2165,7 +2165,7 @@
         <v>24</v>
       </c>
       <c r="I18" s="19">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="J18" s="16" t="s">
         <v>90</v>
@@ -2196,7 +2196,7 @@
         <v>24</v>
       </c>
       <c r="I19" s="19">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J19" s="16" t="s">
         <v>90</v>
@@ -2260,7 +2260,7 @@
         <v>10</v>
       </c>
       <c r="I21" s="19">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="J21" s="16" t="s">
         <v>90</v>
@@ -2359,7 +2359,7 @@
         <v>24</v>
       </c>
       <c r="I24" s="19">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="J24" s="16" t="s">
         <v>93</v>
@@ -2392,7 +2392,7 @@
         <v>24</v>
       </c>
       <c r="I25" s="19">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="J25" s="16" t="s">
         <v>93</v>
@@ -2425,7 +2425,7 @@
         <v>24</v>
       </c>
       <c r="I26" s="19">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="J26" s="16" t="s">
         <v>93</v>
@@ -2458,7 +2458,7 @@
         <v>24</v>
       </c>
       <c r="I27" s="19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J27" s="16" t="s">
         <v>93</v>
@@ -2524,7 +2524,7 @@
         <v>24</v>
       </c>
       <c r="I29" s="19">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="J29" s="16" t="s">
         <v>80</v>
@@ -2557,7 +2557,7 @@
         <v>44</v>
       </c>
       <c r="I30" s="19">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="J30" s="16" t="s">
         <v>97</v>
@@ -2590,7 +2590,7 @@
         <v>6</v>
       </c>
       <c r="I31" s="19">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="J31" s="16" t="s">
         <v>77</v>
@@ -2751,7 +2751,7 @@
         <v>10</v>
       </c>
       <c r="I36" s="19">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J36" s="16" t="s">
         <v>104</v>
@@ -2784,7 +2784,7 @@
         <v>8</v>
       </c>
       <c r="I37" s="19">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J37" s="16" t="s">
         <v>106</v>
@@ -2817,7 +2817,7 @@
         <v>10</v>
       </c>
       <c r="I38" s="19">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="J38" s="16" t="s">
         <v>80</v>
@@ -3137,7 +3137,7 @@
         <v>22</v>
       </c>
       <c r="I48" s="19">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J48" s="16" t="s">
         <v>76</v>
@@ -3168,7 +3168,7 @@
         <v>44</v>
       </c>
       <c r="I49" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" s="16" t="s">
         <v>109</v>
@@ -3234,7 +3234,7 @@
         <v>103</v>
       </c>
       <c r="I51" s="19">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J51" s="16" t="s">
         <v>87</v>
@@ -3267,7 +3267,7 @@
         <v>103</v>
       </c>
       <c r="I52" s="19">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J52" s="16" t="s">
         <v>87</v>
@@ -3294,7 +3294,7 @@
       </c>
       <c r="I53" s="19">
         <f>AVERAGE(I3:I52)</f>
-        <v>0.7659999999999999</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="J53" s="16"/>
       <c r="K53" s="16"/>

</xml_diff>